<commit_message>
Update Tables file and outermost Readme file
</commit_message>
<xml_diff>
--- a/Analysis/Tables/Tables.xlsx
+++ b/Analysis/Tables/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melvinquashie/Documents/Data Analytics /sql projects/22-23 PL stats analysis/Analysis/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EBD7B3-0F30-3E4A-8E82-CD20617D818B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26968EC3-5B23-884E-8FE8-2C00C089F41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" activeTab="5" xr2:uid="{9543F12D-BC8E-6140-9882-C802333C6CB7}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="540">
   <si>
     <t>links</t>
   </si>
@@ -1653,13 +1653,22 @@
   </si>
   <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>RANK() OVER (ORDER BY (3 * (home_wins + away_wins)) + (home_draws + away_draws) DESC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1682,6 +1691,12 @@
       <sz val="14"/>
       <color rgb="FF3C4043"/>
       <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1732,7 +1747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1745,6 +1760,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2085,15 +2102,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>435428</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>471714</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>145143</xdr:rowOff>
+      <xdr:colOff>36286</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2108,7 +2125,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="16328571" y="598714"/>
+          <a:off x="16364857" y="816429"/>
           <a:ext cx="399143" cy="18143"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2138,15 +2155,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>508001</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>145144</xdr:rowOff>
+      <xdr:colOff>508002</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>145143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>453573</xdr:colOff>
+      <xdr:colOff>489861</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>181431</xdr:rowOff>
+      <xdr:rowOff>181430</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2161,12 +2178,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="9325430" y="3773715"/>
-          <a:ext cx="10178144" cy="3864429"/>
+          <a:off x="9461502" y="3873500"/>
+          <a:ext cx="9942287" cy="3900716"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 267"/>
+            <a:gd name="adj1" fmla="val 183"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -2961,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3187019A-72D2-DC47-8343-5DC82A2F8921}">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4369,7 +4386,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4861,8 +4878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB4C599-DBCF-E24D-91A8-223AE5FEE320}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5340,10 +5357,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0B602D-2533-4C45-96F7-0E5DBE519CC4}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5378,41 +5395,41 @@
     </row>
     <row r="3" spans="1:4" ht="18">
       <c r="A3" s="4" t="s">
-        <v>511</v>
+        <v>537</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>510</v>
+        <v>538</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>539</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18">
       <c r="A4" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>518</v>
+        <v>446</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>529</v>
+        <v>510</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18">
       <c r="A5" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>41</v>
@@ -5420,13 +5437,13 @@
     </row>
     <row r="6" spans="1:4" ht="18">
       <c r="A6" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
@@ -5434,13 +5451,13 @@
     </row>
     <row r="7" spans="1:4" ht="18">
       <c r="A7" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>41</v>
@@ -5448,13 +5465,13 @@
     </row>
     <row r="8" spans="1:4" ht="18">
       <c r="A8" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>41</v>
@@ -5462,15 +5479,29 @@
     </row>
     <row r="9" spans="1:4" ht="18">
       <c r="A9" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18">
+      <c r="A10" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5488,7 +5519,7 @@
   <dimension ref="A1:R126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="L3" sqref="L3:L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5568,11 +5599,9 @@
       <c r="L3" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>511</v>
+      <c r="N3" s="2"/>
+      <c r="O3" s="11" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -5591,8 +5620,11 @@
       <c r="L4" s="4" t="s">
         <v>416</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>536</v>
+      </c>
       <c r="O4" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -5609,7 +5641,7 @@
         <v>417</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -5626,7 +5658,7 @@
         <v>418</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -5649,7 +5681,7 @@
         <v>419</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -5666,7 +5698,7 @@
         <v>420</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -5686,7 +5718,7 @@
         <v>421</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -5702,6 +5734,9 @@
       <c r="L10" s="4" t="s">
         <v>422</v>
       </c>
+      <c r="O10" s="4" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="11" spans="1:18">
       <c r="B11" s="4" t="s">
@@ -6546,6 +6581,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Readme and add extracted results
</commit_message>
<xml_diff>
--- a/Analysis/Tables/Tables.xlsx
+++ b/Analysis/Tables/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melvinquashie/Documents/Data Analytics /sql projects/22-23 PL stats analysis/Analysis/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26968EC3-5B23-884E-8FE8-2C00C089F41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8808991-9569-4C41-9EAE-1CDB3FA436DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16480" activeTab="5" xr2:uid="{9543F12D-BC8E-6140-9882-C802333C6CB7}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <sheet name="ERD" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1747,21 +1746,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2519,11 +2516,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -2991,11 +2988,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
@@ -4397,11 +4394,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
@@ -4891,12 +4888,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>527</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="18">
       <c r="A2" s="3" t="s">
@@ -5372,12 +5369,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="18">
       <c r="A2" s="3" t="s">
@@ -5400,7 +5397,7 @@
       <c r="B3" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>539</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -5519,7 +5516,7 @@
   <dimension ref="A1:R126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L33"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5544,27 +5541,27 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="7" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="7" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18">
       <c r="B2" s="3" t="s">
@@ -5573,13 +5570,13 @@
       <c r="F2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="6" t="s">
         <v>524</v>
       </c>
     </row>
@@ -5600,7 +5597,7 @@
         <v>411</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="8" t="s">
         <v>537</v>
       </c>
     </row>
@@ -5668,7 +5665,7 @@
       <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>536</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -5688,6 +5685,7 @@
       <c r="B8" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
@@ -5705,7 +5703,7 @@
       <c r="B9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>536</v>
       </c>
       <c r="F9" s="4" t="s">

</xml_diff>